<commit_message>
update MILP model and output
</commit_message>
<xml_diff>
--- a/Delay Model/OutPut/ec_congestion.xlsx
+++ b/Delay Model/OutPut/ec_congestion.xlsx
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,7 +373,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -444,7 +440,7 @@
         <v>0.5</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E4">
         <v>0.5</v>
@@ -478,7 +474,7 @@
         <v>0.6</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E6">
         <v>0.6</v>

</xml_diff>